<commit_message>
working on MAR goal and CP goal, added data, function is not recogniznig layers, error in configure_toolbox
</commit_message>
<xml_diff>
--- a/prep/HAB/hab_beaches_extent_troubleshooting.xlsx
+++ b/prep/HAB/hab_beaches_extent_troubleshooting.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="165" yWindow="-165" windowWidth="27795" windowHeight="11820"/>
+    <workbookView xWindow="-165" yWindow="6285" windowWidth="27795" windowHeight="11820"/>
   </bookViews>
   <sheets>
     <sheet name="hab_beaches_extent" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
   <si>
     <t>rgn_id</t>
   </si>
@@ -64,13 +64,10 @@
     <t>count</t>
   </si>
   <si>
-    <t>sq meters</t>
-  </si>
-  <si>
-    <t>area</t>
-  </si>
-  <si>
     <t>should be ~220 km</t>
+  </si>
+  <si>
+    <t>km_USGS</t>
   </si>
 </sst>
 </file>
@@ -899,10 +896,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J15"/>
+  <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -910,7 +907,7 @@
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -938,8 +935,11 @@
       <c r="J1" t="s">
         <v>5</v>
       </c>
+      <c r="M1" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2</v>
       </c>
@@ -952,6 +952,10 @@
       <c r="D2">
         <v>1446065.2</v>
       </c>
+      <c r="F2">
+        <f>D2/10000</f>
+        <v>144.60651999999999</v>
+      </c>
       <c r="H2">
         <v>357.33049310000001</v>
       </c>
@@ -961,8 +965,11 @@
       <c r="J2" t="s">
         <v>7</v>
       </c>
+      <c r="M2">
+        <v>90</v>
+      </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -975,6 +982,10 @@
       <c r="D3">
         <v>213166.1</v>
       </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F7" si="0">D3/10000</f>
+        <v>21.316610000000001</v>
+      </c>
       <c r="H3">
         <v>52.674490489999997</v>
       </c>
@@ -985,7 +996,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -998,6 +1009,10 @@
       <c r="D4">
         <v>1333059.8</v>
       </c>
+      <c r="F4">
+        <f t="shared" si="0"/>
+        <v>133.30598000000001</v>
+      </c>
       <c r="H4">
         <v>329.40625060000002</v>
       </c>
@@ -1008,7 +1023,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1021,6 +1036,10 @@
       <c r="D5">
         <v>998064</v>
       </c>
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>99.806399999999996</v>
+      </c>
       <c r="H5">
         <v>246.62698560000001</v>
       </c>
@@ -1030,8 +1049,11 @@
       <c r="J5" t="s">
         <v>7</v>
       </c>
+      <c r="M5">
+        <v>107</v>
+      </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1047,6 +1069,10 @@
       <c r="E6">
         <v>294515</v>
       </c>
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>73.387010000000004</v>
+      </c>
       <c r="H6">
         <v>181.3432511</v>
       </c>
@@ -1056,8 +1082,11 @@
       <c r="J6" t="s">
         <v>7</v>
       </c>
+      <c r="M6">
+        <v>75</v>
+      </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1</v>
       </c>
@@ -1070,6 +1099,10 @@
       <c r="D7">
         <v>62853.1</v>
       </c>
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>6.28531</v>
+      </c>
       <c r="H7">
         <v>15.531339259999999</v>
       </c>
@@ -1080,49 +1113,19 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="F8">
+        <f>SUM(F2:F7)</f>
+        <v>478.70782999999994</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D11">
-        <f>SUM(D2:D7)</f>
-        <v>4787078.3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C13" t="s">
-        <v>15</v>
-      </c>
-      <c r="D13" t="s">
         <v>16</v>
       </c>
-      <c r="F13" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C14">
-        <v>2481457</v>
-      </c>
-      <c r="D14">
-        <f>C14*(2.4*2.4)</f>
-        <v>14293192.32</v>
-      </c>
-      <c r="F14">
-        <f>D14/1000000</f>
-        <v>14.293192320000001</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C15">
-        <f>C14/1000000</f>
-        <v>2.4814569999999998</v>
-      </c>
-      <c r="D15">
-        <f>D14/D11</f>
-        <v>2.9857861986506467</v>
+      <c r="F9">
+        <f>F8/1000</f>
+        <v>0.47870782999999995</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Data collection and organization for HAB and SPP
</commit_message>
<xml_diff>
--- a/prep/HAB/hab_beaches_extent_troubleshooting.xlsx
+++ b/prep/HAB/hab_beaches_extent_troubleshooting.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-165" yWindow="6285" windowWidth="27795" windowHeight="11820"/>
+    <workbookView xWindow="-8310" yWindow="6195" windowWidth="27795" windowHeight="11820"/>
   </bookViews>
   <sheets>
     <sheet name="hab_beaches_extent" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -899,7 +899,7 @@
   <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>